<commit_message>
update helper_AmazonEC2.md, 4.2. Data Transfer
</commit_message>
<xml_diff>
--- a/AWS/cost-IPv4andNAT-GW.xlsx
+++ b/AWS/cost-IPv4andNAT-GW.xlsx
@@ -31,16 +31,16 @@
     <t xml:space="preserve">EC2 + NAT GW</t>
   </si>
   <si>
-    <t xml:space="preserve">小計</t>
-  </si>
-  <si>
-    <t xml:space="preserve">每小時</t>
-  </si>
-  <si>
-    <t xml:space="preserve">小時</t>
-  </si>
-  <si>
-    <t xml:space="preserve">月</t>
+    <t xml:space="preserve">SUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$/hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hour(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">month(s)</t>
   </si>
   <si>
     <t xml:space="preserve">Public IPv4</t>
@@ -49,27 +49,10 @@
     <t xml:space="preserve">NAT GW </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <rFont val="Noto Sans TC"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t xml:space="preserve">每</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="15"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="136"/>
-      </rPr>
-      <t xml:space="preserve">GB</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">GB</t>
+    <t xml:space="preserve">$/GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GB(s)</t>
   </si>
   <si>
     <t xml:space="preserve">NAT GW → Internet</t>
@@ -98,7 +81,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Noto Sans TC"/>
@@ -125,12 +108,12 @@
     </font>
     <font>
       <sz val="15"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
+      <name val="Noto Sans TC"/>
+      <family val="2"/>
+      <charset val="136"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="15"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -141,18 +124,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <name val="Noto Sans TC"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="136"/>
     </font>
   </fonts>
   <fills count="7">
@@ -234,7 +205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -255,11 +226,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -271,7 +242,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -279,15 +262,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -375,24 +358,24 @@
   <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O17" activeCellId="0" sqref="O17"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.3125" defaultRowHeight="18.55" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="7.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="12.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="4" width="3.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="9.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="17.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="12.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="12.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="4" width="3.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="9.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="17.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="12.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="12.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="3.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="6.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="20.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="12.07"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="12.31"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="14" style="5" width="12.31"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="27" min="27" style="6" width="12.31"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="28" style="3" width="12.31"/>
@@ -401,17 +384,20 @@
     <row r="1" s="8" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="7"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="8" t="s">
-        <v>0</v>
-      </c>
+      <c r="F1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="9"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>1</v>
       </c>
+      <c r="J1" s="9"/>
       <c r="K1" s="4"/>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="M1" s="9"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -428,21 +414,21 @@
       <c r="AA1" s="6"/>
     </row>
     <row r="2" s="8" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="G2" s="9" t="n">
+      <c r="G2" s="11" t="n">
         <f aca="false">SUM(G3:G23)</f>
         <v>36.77</v>
       </c>
       <c r="H2" s="4"/>
-      <c r="J2" s="9" t="n">
+      <c r="J2" s="11" t="n">
         <f aca="false">SUM(J3:J23)</f>
         <v>3.92</v>
       </c>
       <c r="K2" s="4"/>
-      <c r="M2" s="9" t="n">
+      <c r="M2" s="11" t="n">
         <f aca="false">SUM(M3:M23)</f>
         <v>36.635</v>
       </c>
@@ -463,22 +449,22 @@
     </row>
     <row r="3" s="2" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="4"/>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="12" t="s">
         <v>6</v>
       </c>
       <c r="N3" s="5"/>
@@ -497,10 +483,10 @@
       <c r="AA3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10" t="n">
+      <c r="B4" s="13" t="n">
         <v>0.005</v>
       </c>
       <c r="C4" s="3" t="n">
@@ -533,11 +519,11 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="n">
@@ -559,41 +545,41 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
+      <c r="A7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-    </row>
-    <row r="9" s="12" customFormat="true" ht="19.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" s="16" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="12" t="s">
         <v>10</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="2" t="s">
+      <c r="L9" s="12" t="s">
         <v>10</v>
       </c>
       <c r="M9" s="2"/>
@@ -613,7 +599,7 @@
       <c r="AA9" s="6"/>
     </row>
     <row r="10" s="2" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2" t="n">
@@ -656,7 +642,7 @@
       <c r="AA10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="n">
@@ -678,7 +664,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2" t="n">
@@ -700,7 +686,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2" t="n">
@@ -729,40 +715,40 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
     </row>
     <row r="18" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="12" t="s">
         <v>6</v>
       </c>
       <c r="G18" s="2"/>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="12" t="s">
         <v>6</v>
       </c>
       <c r="J18" s="2"/>
-      <c r="L18" s="2" t="s">
+      <c r="L18" s="12" t="s">
         <v>6</v>
       </c>
       <c r="M18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="2" t="n">
@@ -783,27 +769,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" s="12" customFormat="true" ht="19.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="16" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="12" t="s">
         <v>10</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="2" t="s">
+      <c r="L20" s="12" t="s">
         <v>10</v>
       </c>
       <c r="M20" s="2"/>
@@ -823,7 +809,7 @@
       <c r="AA20" s="6"/>
     </row>
     <row r="21" s="2" customFormat="true" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B21" s="2" t="n">
@@ -894,7 +880,7 @@
       <c r="AA23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>

</xml_diff>